<commit_message>
Fixing typos in organoids field names
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_experiment.xlsx
+++ b/src/assets/empty/faang_experiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95E349F-7C0E-6347-962E-4D664BD3E541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9844A9F-709E-054F-8468-A11C88C54A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="8" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{58DBCFEB-F75F-A348-9496-13E962F9C8F7}"/>
   </bookViews>
   <sheets>
     <sheet name="submission" sheetId="13" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="324">
   <si>
     <t>Sample Descriptor</t>
   </si>
@@ -1018,6 +1018,9 @@
   </si>
   <si>
     <t>Adapter Step</t>
+  </si>
+  <si>
+    <t>NextSeq 2000</t>
   </si>
 </sst>
 </file>
@@ -2522,10 +2525,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFC3F93-CB0B-BF48-9B11-5793D4DCF38D}">
-  <dimension ref="A1:BB1000"/>
+  <dimension ref="A1:BC1000"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="BC17" sqref="BC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3039,7 +3042,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>196</v>
       </c>
@@ -3202,8 +3205,11 @@
       <c r="BB17" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="18" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BC17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>261</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>263</v>
       </c>
@@ -3258,7 +3264,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>277</v>
       </c>
@@ -3332,18 +3338,18 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4313,7 +4319,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nbWpHRhNtjHyFXOZcT4N3EthZhZMpDuczJXk7PosX/sQ7EW8HBDaLBnNNwFiHRFv4EislTLdsF92vPYw6qcRyg==" saltValue="MrfqNx8AqNkPXQSuiEXwSw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="sAuiyFEGJJ1sKigCSPZwC7GiIGVLwfMRquQSiZucDzFMEd4LyTzcSo4jqfoCzIgaCzI1iNGljxasutRFlvdT1A==" saltValue="99lYszZxeigXcrEyiP+b9Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4474,8 +4480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F098638-7041-8742-A382-2ACA2B20888B}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5569,7 +5575,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{8A85B586-78C5-3A4F-82C3-CA4CF7CE4605}">
           <x14:formula1>
             <xm:f>faang_field_values!$A$12:$AJ$12</xm:f>
@@ -5604,7 +5610,13 @@
           <x14:formula1>
             <xm:f>faang_field_values!$A$17:$BB$17</xm:f>
           </x14:formula1>
-          <xm:sqref>O3:O61 O2</xm:sqref>
+          <xm:sqref>O3:O61</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{6E48A385-1211-CF4E-8AE0-ACA32D191723}">
+          <x14:formula1>
+            <xm:f>faang_field_values!$A$17:$BC$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8545,7 +8557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BD49F3-4725-E748-A029-B6B285E09FD7}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>

</xml_diff>